<commit_message>
early results from borrowing constraint model
</commit_message>
<xml_diff>
--- a/Examples/BorrowingConstraint/Results.xlsx
+++ b/Examples/BorrowingConstraint/Results.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dynare\dynareOBC\Examples\CapitalConstraints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dynare\dynareOBC\Examples\BorrowingConstraint\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14175" windowHeight="6825" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14175" windowHeight="6825" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Source Data" sheetId="3" r:id="rId1"/>
+    <sheet name="Data for 1 Norm Plot" sheetId="1" r:id="rId2"/>
+    <sheet name="1 Norm Plot" sheetId="2" r:id="rId3"/>
+    <sheet name="Data for Inf Norm Plot" sheetId="4" r:id="rId4"/>
+    <sheet name="Inf Norm Plot" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>1023 point QMC</t>
   </si>
@@ -34,6 +37,18 @@
   </si>
   <si>
     <t>Periods of uncertainty</t>
+  </si>
+  <si>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>QMC 9</t>
+  </si>
+  <si>
+    <t>Horizon</t>
+  </si>
+  <si>
+    <t>Infinity</t>
   </si>
 </sst>
 </file>
@@ -80,9 +95,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -126,7 +144,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>'Data for 1 Norm Plot'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -161,7 +179,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$45</c:f>
+              <c:f>'Data for 1 Norm Plot'!$A$2:$A$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
@@ -227,78 +245,150 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$45</c:f>
+              <c:f>'Data for 1 Norm Plot'!$B$2:$B$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
                 <c:pt idx="0">
-                  <c:v>5.6904418568273502E-4</c:v>
+                  <c:v>3.7400816402754201E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.2944255760436197E-4</c:v>
+                  <c:v>3.3101219461231898E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1578700705044798E-4</c:v>
+                  <c:v>3.17357351106775E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9477195682145103E-4</c:v>
+                  <c:v>3.0520631703134398E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.75342296195695E-4</c:v>
+                  <c:v>2.9526597785378499E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.6195835580417301E-4</c:v>
+                  <c:v>2.7276737473014099E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.53484151319983E-4</c:v>
+                  <c:v>2.6248750420700198E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.4826916223397999E-4</c:v>
+                  <c:v>2.53493561805801E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.4833848388715398E-4</c:v>
+                  <c:v>2.4572763717441801E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.4978592856210299E-4</c:v>
+                  <c:v>2.3912575844339101E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.48147731166954E-4</c:v>
+                  <c:v>2.33478952330172E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.4823610235986301E-4</c:v>
+                  <c:v>2.2873168637966498E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.4977107010801403E-4</c:v>
+                  <c:v>2.2476006556273798E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.4717588217279398E-4</c:v>
+                  <c:v>2.2147437892379002E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.4810924483685801E-4</c:v>
+                  <c:v>2.18761406320034E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.49908097391499E-4</c:v>
+                  <c:v>2.1649856337734698E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.5238188822885903E-4</c:v>
+                  <c:v>2.1473849503767699E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.5354170216847502E-4</c:v>
+                  <c:v>2.1345084948281002E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.5297381082394099E-4</c:v>
+                  <c:v>1.81339003812334E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.5282695583581802E-4</c:v>
+                  <c:v>1.7924257212901199E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.5427588803260402E-4</c:v>
+                  <c:v>1.77537107833506E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.76211607944527E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.7521251302226001E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.7449411465290999E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.7399484028263301E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.7377591829206901E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.73764346141537E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.7393559662726701E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.74262559523878E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.74708544199504E-3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.7530586585770801E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.75996581163959E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.76805888780284E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -315,7 +405,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>'Data for 1 Norm Plot'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -351,7 +441,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$45</c:f>
+              <c:f>'Data for 1 Norm Plot'!$A$2:$A$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
@@ -417,78 +507,150 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$45</c:f>
+              <c:f>'Data for 1 Norm Plot'!$C$2:$C$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
                 <c:pt idx="0">
-                  <c:v>5.6904418568273502E-4</c:v>
+                  <c:v>3.7400816402754201E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.3050905030278199E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.19859487883361E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0995797084665601E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0326271577093404E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.9868754529179798E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.95826726444864E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.9205469366551697E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.9205628982074904E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.8769062905559899E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.8592273531398902E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.8744769957511199E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.8543132342882298E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.8413807643665801E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.8296661124961699E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.8431360069960101E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.8555376115622697E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.8674513934886401E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.8375800241109101E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.8458041232137401E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.8420744756603199E-4</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -515,7 +677,7 @@
         <c:axId val="192072752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="20"/>
+          <c:max val="32"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -640,8 +802,878 @@
         <c:axId val="192063184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="5.8000000000000011E-4"/>
-          <c:min val="4.4000000000000012E-4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Mean absolute error</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> in log consumption</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="192072752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data for Inf Norm Plot'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Degree 3 monomial rule</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Data for Inf Norm Plot'!$A$2:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="44"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Data for Inf Norm Plot'!$B$2:$B$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="44"/>
+                <c:pt idx="0">
+                  <c:v>1.9767040447665099E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6928848208210199E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5714586582483099E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4701835465686401E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.36996738653679E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.25066552214577E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.17118586178135E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.10228615121051E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.04450141389481E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.00031128984164E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.6456023373340805E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.3013692262083301E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.9861094033244493E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.6608779937408006E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.3676129656934401E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.1064583102366805E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.8913277685779808E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.5567778944868897E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.3420692093071104E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.1236174390905699E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.8118158929674202E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.4786820946310403E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.1032063856742104E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.7435560147693398E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.4437287006837099E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.18547558561028E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.9429763099456403E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.7249947053956401E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.5459482564271202E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.4220377076199203E-3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.32236991034238E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.35544275047944E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.4312218192159598E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-22C1-4CFF-B94F-50CEE5F903EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data for Inf Norm Plot'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1023 point QMC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="lgDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Data for Inf Norm Plot'!$A$2:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="44"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Data for Inf Norm Plot'!$C$2:$C$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="44"/>
+                <c:pt idx="0">
+                  <c:v>1.9767040447665099E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-22C1-4CFF-B94F-50CEE5F903EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="192072752"/>
+        <c:axId val="192063184"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="192072752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="32"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Periods</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> of future uncertainty considered</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="192063184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="4"/>
+        <c:minorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="192063184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -858,6 +1890,33 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
+  <cs:variation>
+    <a:tint val="88500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="55000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="75000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="98500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="80000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1374,11 +2433,538 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1389,7 +2975,34 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9293087" cy="6079435"/>
+    <xdr:ext cx="9298983" cy="6078242"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9298983" cy="6078242"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1488,6 +3101,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1523,6 +3153,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1675,15 +3322,544 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>3.7400816402754201E-3</v>
+      </c>
+      <c r="C3">
+        <v>6.4881998810249301E-3</v>
+      </c>
+      <c r="D3">
+        <v>1.9767040447665099E-2</v>
+      </c>
+      <c r="E3">
+        <v>3.7400816402754201E-3</v>
+      </c>
+      <c r="F3">
+        <v>6.4881998810249301E-3</v>
+      </c>
+      <c r="G3">
+        <v>1.9767040447665099E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3.3101219461231898E-3</v>
+      </c>
+      <c r="C4">
+        <v>5.4090219060962596E-3</v>
+      </c>
+      <c r="D4">
+        <v>1.6928848208210199E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>3.17357351106775E-3</v>
+      </c>
+      <c r="C5">
+        <v>5.0675512046483503E-3</v>
+      </c>
+      <c r="D5">
+        <v>1.5714586582483099E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>3.0520631703134398E-3</v>
+      </c>
+      <c r="C6">
+        <v>4.7717073288979497E-3</v>
+      </c>
+      <c r="D6">
+        <v>1.4701835465686401E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>2.9526597785378499E-3</v>
+      </c>
+      <c r="C7">
+        <v>4.5304497502403496E-3</v>
+      </c>
+      <c r="D7">
+        <v>1.36996738653679E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>2.7276737473014099E-3</v>
+      </c>
+      <c r="C8">
+        <v>4.0995894893176999E-3</v>
+      </c>
+      <c r="D8">
+        <v>1.25066552214577E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>2.6248750420700198E-3</v>
+      </c>
+      <c r="C9">
+        <v>3.8722881474278601E-3</v>
+      </c>
+      <c r="D9">
+        <v>1.17118586178135E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>2.53493561805801E-3</v>
+      </c>
+      <c r="C10">
+        <v>3.6757656242418402E-3</v>
+      </c>
+      <c r="D10">
+        <v>1.10228615121051E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>2.4572763717441801E-3</v>
+      </c>
+      <c r="C11">
+        <v>3.5067337096386002E-3</v>
+      </c>
+      <c r="D11">
+        <v>1.04450141389481E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>2.3912575844339101E-3</v>
+      </c>
+      <c r="C12">
+        <v>3.3638442099469998E-3</v>
+      </c>
+      <c r="D12">
+        <v>1.00031128984164E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>2.33478952330172E-3</v>
+      </c>
+      <c r="C13">
+        <v>3.24256692152692E-3</v>
+      </c>
+      <c r="D13">
+        <v>9.6456023373340805E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>2.2873168637966498E-3</v>
+      </c>
+      <c r="C14">
+        <v>3.1412647681097099E-3</v>
+      </c>
+      <c r="D14">
+        <v>9.3013692262083301E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>2.2476006556273798E-3</v>
+      </c>
+      <c r="C15">
+        <v>3.0570430192578702E-3</v>
+      </c>
+      <c r="D15">
+        <v>8.9861094033244493E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>2.2147437892379002E-3</v>
+      </c>
+      <c r="C16">
+        <v>2.98723719131949E-3</v>
+      </c>
+      <c r="D16">
+        <v>8.6608779937408006E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>2.18761406320034E-3</v>
+      </c>
+      <c r="C17">
+        <v>2.9288257633514701E-3</v>
+      </c>
+      <c r="D17">
+        <v>8.3676129656934401E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>2.1649856337734698E-3</v>
+      </c>
+      <c r="C18">
+        <v>2.8797575807609698E-3</v>
+      </c>
+      <c r="D18">
+        <v>8.1064583102366805E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>2.1473849503767699E-3</v>
+      </c>
+      <c r="C19">
+        <v>2.8414192826340498E-3</v>
+      </c>
+      <c r="D19">
+        <v>7.8913277685779808E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>2.1345084948281002E-3</v>
+      </c>
+      <c r="C20">
+        <v>2.8133932297788899E-3</v>
+      </c>
+      <c r="D20">
+        <v>7.5567778944868897E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>1.81339003812334E-3</v>
+      </c>
+      <c r="C21">
+        <v>2.30733443388321E-3</v>
+      </c>
+      <c r="D21">
+        <v>7.3420692093071104E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>1.7924257212901199E-3</v>
+      </c>
+      <c r="C22">
+        <v>2.2637524978168298E-3</v>
+      </c>
+      <c r="D22">
+        <v>7.1236174390905699E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>1.77537107833506E-3</v>
+      </c>
+      <c r="C23">
+        <v>2.2280346201456799E-3</v>
+      </c>
+      <c r="D23">
+        <v>6.8118158929674202E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>1.76211607944527E-3</v>
+      </c>
+      <c r="C24">
+        <v>2.1999162272173601E-3</v>
+      </c>
+      <c r="D24">
+        <v>6.4786820946310403E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>1.7521251302226001E-3</v>
+      </c>
+      <c r="C25">
+        <v>2.17882170353425E-3</v>
+      </c>
+      <c r="D25">
+        <v>6.1032063856742104E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>1.7449411465290999E-3</v>
+      </c>
+      <c r="C26">
+        <v>2.1632500772310499E-3</v>
+      </c>
+      <c r="D26">
+        <v>5.7435560147693398E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>1.7399484028263301E-3</v>
+      </c>
+      <c r="C27">
+        <v>2.1521550840283101E-3</v>
+      </c>
+      <c r="D27">
+        <v>5.4437287006837099E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>1.7377591829206901E-3</v>
+      </c>
+      <c r="C28">
+        <v>2.1465894838719E-3</v>
+      </c>
+      <c r="D28">
+        <v>5.18547558561028E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29">
+        <v>1.73764346141537E-3</v>
+      </c>
+      <c r="C29">
+        <v>2.1451555893955698E-3</v>
+      </c>
+      <c r="D29">
+        <v>4.9429763099456403E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <v>1.7393559662726701E-3</v>
+      </c>
+      <c r="C30">
+        <v>2.1470726671506202E-3</v>
+      </c>
+      <c r="D30">
+        <v>4.7249947053956401E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <v>1.74262559523878E-3</v>
+      </c>
+      <c r="C31">
+        <v>2.1518903180695798E-3</v>
+      </c>
+      <c r="D31">
+        <v>4.5459482564271202E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32">
+        <v>1.74708544199504E-3</v>
+      </c>
+      <c r="C32">
+        <v>2.1589301497410302E-3</v>
+      </c>
+      <c r="D32">
+        <v>4.4220377076199203E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33">
+        <v>1.7530586585770801E-3</v>
+      </c>
+      <c r="C33">
+        <v>2.1687948293161001E-3</v>
+      </c>
+      <c r="D33">
+        <v>4.32236991034238E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>1.75996581163959E-3</v>
+      </c>
+      <c r="C34">
+        <v>2.18045528671972E-3</v>
+      </c>
+      <c r="D34">
+        <v>4.35544275047944E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="B35">
+        <v>1.76805888780284E-3</v>
+      </c>
+      <c r="C35">
+        <v>2.1942672410295702E-3</v>
+      </c>
+      <c r="D35">
+        <v>4.4312218192159598E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:C35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1699,10 +3875,12 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5.6904418568273502E-4</v>
+        <f>'Source Data'!B3</f>
+        <v>3.7400816402754201E-3</v>
       </c>
       <c r="C2">
-        <v>5.6904418568273502E-4</v>
+        <f>'Source Data'!E3</f>
+        <v>3.7400816402754201E-3</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -1712,10 +3890,12 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5.2944255760436197E-4</v>
+        <f>'Source Data'!B4</f>
+        <v>3.3101219461231898E-3</v>
       </c>
       <c r="C3">
-        <v>5.3050905030278199E-4</v>
+        <f>'Source Data'!E4</f>
+        <v>0</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1725,10 +3905,12 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5.1578700705044798E-4</v>
+        <f>'Source Data'!B5</f>
+        <v>3.17357351106775E-3</v>
       </c>
       <c r="C4">
-        <v>5.19859487883361E-4</v>
+        <f>'Source Data'!E5</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1736,10 +3918,12 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>4.9477195682145103E-4</v>
+        <f>'Source Data'!B6</f>
+        <v>3.0520631703134398E-3</v>
       </c>
       <c r="C5">
-        <v>5.0995797084665601E-4</v>
+        <f>'Source Data'!E6</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1747,10 +3931,12 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>4.75342296195695E-4</v>
+        <f>'Source Data'!B7</f>
+        <v>2.9526597785378499E-3</v>
       </c>
       <c r="C6">
-        <v>5.0326271577093404E-4</v>
+        <f>'Source Data'!E7</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1758,10 +3944,12 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>4.6195835580417301E-4</v>
+        <f>'Source Data'!B8</f>
+        <v>2.7276737473014099E-3</v>
       </c>
       <c r="C7">
-        <v>4.9868754529179798E-4</v>
+        <f>'Source Data'!E8</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1769,10 +3957,12 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>4.53484151319983E-4</v>
+        <f>'Source Data'!B9</f>
+        <v>2.6248750420700198E-3</v>
       </c>
       <c r="C8">
-        <v>4.95826726444864E-4</v>
+        <f>'Source Data'!E9</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1780,10 +3970,12 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>4.4826916223397999E-4</v>
+        <f>'Source Data'!B10</f>
+        <v>2.53493561805801E-3</v>
       </c>
       <c r="C9">
-        <v>4.9205469366551697E-4</v>
+        <f>'Source Data'!E10</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1791,10 +3983,12 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>4.4833848388715398E-4</v>
+        <f>'Source Data'!B11</f>
+        <v>2.4572763717441801E-3</v>
       </c>
       <c r="C10">
-        <v>4.9205628982074904E-4</v>
+        <f>'Source Data'!E11</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1802,10 +3996,12 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>4.4978592856210299E-4</v>
+        <f>'Source Data'!B12</f>
+        <v>2.3912575844339101E-3</v>
       </c>
       <c r="C11">
-        <v>4.8769062905559899E-4</v>
+        <f>'Source Data'!E12</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1813,10 +4009,12 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>4.48147731166954E-4</v>
+        <f>'Source Data'!B13</f>
+        <v>2.33478952330172E-3</v>
       </c>
       <c r="C12">
-        <v>4.8592273531398902E-4</v>
+        <f>'Source Data'!E13</f>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1824,10 +4022,12 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>4.4823610235986301E-4</v>
+        <f>'Source Data'!B14</f>
+        <v>2.2873168637966498E-3</v>
       </c>
       <c r="C13">
-        <v>4.8744769957511199E-4</v>
+        <f>'Source Data'!E14</f>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1835,10 +4035,12 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>4.4977107010801403E-4</v>
+        <f>'Source Data'!B15</f>
+        <v>2.2476006556273798E-3</v>
       </c>
       <c r="C14">
-        <v>4.8543132342882298E-4</v>
+        <f>'Source Data'!E15</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1846,10 +4048,12 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>4.4717588217279398E-4</v>
+        <f>'Source Data'!B16</f>
+        <v>2.2147437892379002E-3</v>
       </c>
       <c r="C15">
-        <v>4.8413807643665801E-4</v>
+        <f>'Source Data'!E16</f>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1857,10 +4061,12 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>4.4810924483685801E-4</v>
+        <f>'Source Data'!B17</f>
+        <v>2.18761406320034E-3</v>
       </c>
       <c r="C16">
-        <v>4.8296661124961699E-4</v>
+        <f>'Source Data'!E17</f>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1868,10 +4074,12 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>4.49908097391499E-4</v>
+        <f>'Source Data'!B18</f>
+        <v>2.1649856337734698E-3</v>
       </c>
       <c r="C17">
-        <v>4.8431360069960101E-4</v>
+        <f>'Source Data'!E18</f>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1879,10 +4087,12 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>4.5238188822885903E-4</v>
+        <f>'Source Data'!B19</f>
+        <v>2.1473849503767699E-3</v>
       </c>
       <c r="C18">
-        <v>4.8555376115622697E-4</v>
+        <f>'Source Data'!E19</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1890,10 +4100,12 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>4.5354170216847502E-4</v>
+        <f>'Source Data'!B20</f>
+        <v>2.1345084948281002E-3</v>
       </c>
       <c r="C19">
-        <v>4.8674513934886401E-4</v>
+        <f>'Source Data'!E20</f>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1901,10 +4113,12 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>4.5297381082394099E-4</v>
+        <f>'Source Data'!B21</f>
+        <v>1.81339003812334E-3</v>
       </c>
       <c r="C20">
-        <v>4.8375800241109101E-4</v>
+        <f>'Source Data'!E21</f>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1912,10 +4126,12 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>4.5282695583581802E-4</v>
+        <f>'Source Data'!B22</f>
+        <v>1.7924257212901199E-3</v>
       </c>
       <c r="C21">
-        <v>4.8458041232137401E-4</v>
+        <f>'Source Data'!E22</f>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1923,10 +4139,631 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>4.5427588803260402E-4</v>
+        <f>'Source Data'!B23</f>
+        <v>1.77537107833506E-3</v>
       </c>
       <c r="C22">
-        <v>4.8420744756603199E-4</v>
+        <f>'Source Data'!E23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <f>'Source Data'!B24</f>
+        <v>1.76211607944527E-3</v>
+      </c>
+      <c r="C23">
+        <f>'Source Data'!E24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <f>'Source Data'!B25</f>
+        <v>1.7521251302226001E-3</v>
+      </c>
+      <c r="C24">
+        <f>'Source Data'!E25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <f>'Source Data'!B26</f>
+        <v>1.7449411465290999E-3</v>
+      </c>
+      <c r="C25">
+        <f>'Source Data'!E26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <f>'Source Data'!B27</f>
+        <v>1.7399484028263301E-3</v>
+      </c>
+      <c r="C26">
+        <f>'Source Data'!E27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <f>'Source Data'!B28</f>
+        <v>1.7377591829206901E-3</v>
+      </c>
+      <c r="C27">
+        <f>'Source Data'!E28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <f>'Source Data'!B29</f>
+        <v>1.73764346141537E-3</v>
+      </c>
+      <c r="C28">
+        <f>'Source Data'!E29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <f>'Source Data'!B30</f>
+        <v>1.7393559662726701E-3</v>
+      </c>
+      <c r="C29">
+        <f>'Source Data'!E30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <f>'Source Data'!B31</f>
+        <v>1.74262559523878E-3</v>
+      </c>
+      <c r="C30">
+        <f>'Source Data'!E31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <f>'Source Data'!B32</f>
+        <v>1.74708544199504E-3</v>
+      </c>
+      <c r="C31">
+        <f>'Source Data'!E32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <f>'Source Data'!B33</f>
+        <v>1.7530586585770801E-3</v>
+      </c>
+      <c r="C32">
+        <f>'Source Data'!E33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <f>'Source Data'!B34</f>
+        <v>1.75996581163959E-3</v>
+      </c>
+      <c r="C33">
+        <f>'Source Data'!E34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <f>'Source Data'!B35</f>
+        <v>1.76805888780284E-3</v>
+      </c>
+      <c r="C34">
+        <f>'Source Data'!E35</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>'Source Data'!D3</f>
+        <v>1.9767040447665099E-2</v>
+      </c>
+      <c r="C2">
+        <f>'Source Data'!G3</f>
+        <v>1.9767040447665099E-2</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f>'Source Data'!D4</f>
+        <v>1.6928848208210199E-2</v>
+      </c>
+      <c r="C3">
+        <f>'Source Data'!G4</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f>'Source Data'!D5</f>
+        <v>1.5714586582483099E-2</v>
+      </c>
+      <c r="C4">
+        <f>'Source Data'!G5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <f>'Source Data'!D6</f>
+        <v>1.4701835465686401E-2</v>
+      </c>
+      <c r="C5">
+        <f>'Source Data'!G6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <f>'Source Data'!D7</f>
+        <v>1.36996738653679E-2</v>
+      </c>
+      <c r="C6">
+        <f>'Source Data'!G7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <f>'Source Data'!D8</f>
+        <v>1.25066552214577E-2</v>
+      </c>
+      <c r="C7">
+        <f>'Source Data'!G8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f>'Source Data'!D9</f>
+        <v>1.17118586178135E-2</v>
+      </c>
+      <c r="C8">
+        <f>'Source Data'!G9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <f>'Source Data'!D10</f>
+        <v>1.10228615121051E-2</v>
+      </c>
+      <c r="C9">
+        <f>'Source Data'!G10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <f>'Source Data'!D11</f>
+        <v>1.04450141389481E-2</v>
+      </c>
+      <c r="C10">
+        <f>'Source Data'!G11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f>'Source Data'!D12</f>
+        <v>1.00031128984164E-2</v>
+      </c>
+      <c r="C11">
+        <f>'Source Data'!G12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <f>'Source Data'!D13</f>
+        <v>9.6456023373340805E-3</v>
+      </c>
+      <c r="C12">
+        <f>'Source Data'!G13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f>'Source Data'!D14</f>
+        <v>9.3013692262083301E-3</v>
+      </c>
+      <c r="C13">
+        <f>'Source Data'!G14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f>'Source Data'!D15</f>
+        <v>8.9861094033244493E-3</v>
+      </c>
+      <c r="C14">
+        <f>'Source Data'!G15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <f>'Source Data'!D16</f>
+        <v>8.6608779937408006E-3</v>
+      </c>
+      <c r="C15">
+        <f>'Source Data'!G16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <f>'Source Data'!D17</f>
+        <v>8.3676129656934401E-3</v>
+      </c>
+      <c r="C16">
+        <f>'Source Data'!G17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <f>'Source Data'!D18</f>
+        <v>8.1064583102366805E-3</v>
+      </c>
+      <c r="C17">
+        <f>'Source Data'!G18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <f>'Source Data'!D19</f>
+        <v>7.8913277685779808E-3</v>
+      </c>
+      <c r="C18">
+        <f>'Source Data'!G19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <f>'Source Data'!D20</f>
+        <v>7.5567778944868897E-3</v>
+      </c>
+      <c r="C19">
+        <f>'Source Data'!G20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <f>'Source Data'!D21</f>
+        <v>7.3420692093071104E-3</v>
+      </c>
+      <c r="C20">
+        <f>'Source Data'!G21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <f>'Source Data'!D22</f>
+        <v>7.1236174390905699E-3</v>
+      </c>
+      <c r="C21">
+        <f>'Source Data'!G22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <f>'Source Data'!D23</f>
+        <v>6.8118158929674202E-3</v>
+      </c>
+      <c r="C22">
+        <f>'Source Data'!G23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <f>'Source Data'!D24</f>
+        <v>6.4786820946310403E-3</v>
+      </c>
+      <c r="C23">
+        <f>'Source Data'!G24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <f>'Source Data'!D25</f>
+        <v>6.1032063856742104E-3</v>
+      </c>
+      <c r="C24">
+        <f>'Source Data'!G25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <f>'Source Data'!D26</f>
+        <v>5.7435560147693398E-3</v>
+      </c>
+      <c r="C25">
+        <f>'Source Data'!G26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <f>'Source Data'!D27</f>
+        <v>5.4437287006837099E-3</v>
+      </c>
+      <c r="C26">
+        <f>'Source Data'!G27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <f>'Source Data'!D28</f>
+        <v>5.18547558561028E-3</v>
+      </c>
+      <c r="C27">
+        <f>'Source Data'!G28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <f>'Source Data'!D29</f>
+        <v>4.9429763099456403E-3</v>
+      </c>
+      <c r="C28">
+        <f>'Source Data'!G29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <f>'Source Data'!D30</f>
+        <v>4.7249947053956401E-3</v>
+      </c>
+      <c r="C29">
+        <f>'Source Data'!G30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <f>'Source Data'!D31</f>
+        <v>4.5459482564271202E-3</v>
+      </c>
+      <c r="C30">
+        <f>'Source Data'!G31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <f>'Source Data'!D32</f>
+        <v>4.4220377076199203E-3</v>
+      </c>
+      <c r="C31">
+        <f>'Source Data'!G32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <f>'Source Data'!D33</f>
+        <v>4.32236991034238E-3</v>
+      </c>
+      <c r="C32">
+        <f>'Source Data'!G33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <f>'Source Data'!D34</f>
+        <v>4.35544275047944E-3</v>
+      </c>
+      <c r="C33">
+        <f>'Source Data'!G34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <f>'Source Data'!D35</f>
+        <v>4.4312218192159598E-3</v>
+      </c>
+      <c r="C34">
+        <f>'Source Data'!G35</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix graph axis labels
</commit_message>
<xml_diff>
--- a/Examples/BorrowingConstraint/Results.xlsx
+++ b/Examples/BorrowingConstraint/Results.xlsx
@@ -19,6 +19,7 @@
     <sheet name="Inf Norm Plot" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -844,7 +845,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> in log consumption</a:t>
+                  <a:t> in X=C+D</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -1711,12 +1712,10 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Mean absolute error</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> in log consumption</a:t>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Maximum absolute error in X=C+D</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>

</xml_diff>